<commit_message>
Execute All GSM Test Cases.
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="61">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -89,23 +89,157 @@
     <t>Error Handling - GSM_ERROR_HTTP_SERVER_ERROR</t>
   </si>
   <si>
-    <t>For any HHTP status other than 200:
+    <t>Retransmits the data</t>
+  </si>
+  <si>
+    <t>GPS MTK3339 Module</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Observation Details</t>
+  </si>
+  <si>
+    <t>Stuck at APP_HANDLE_ERROR : GSM_ERROR_DEV_ACK</t>
+  </si>
+  <si>
+    <t>Usart read error shows rendomly when µC try to read CMD_ACK. Prints only "APP_HANDLE_ERROR: GSM_ERROR_DEV_ACK". There are no Error handling form Application's side. Getting Error ACK message,at AT+CSTT="www","","". Getting error ack message after running GPS init(block) 7 times at interval of 10sec.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Observation count = 258, Usart read error shows rendomly. If allocate_and_copy_urls(); calls more than 120 times at 'GSM_HTTP_HTTP_INIT', then µC return </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>General Exception Data bus error (cause=7, addr=9d0179b8).</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Usart read error rendomly, General Exception</t>
+  </si>
+  <si>
+    <t>Allocate required memory
+Init USART
+Sends sequence of AT commands and receive the responses</t>
+  </si>
+  <si>
+    <t>GSM_GPRS_BASIC init Success</t>
+  </si>
+  <si>
+    <t>GSM_HTTP_INIT success</t>
+  </si>
+  <si>
+    <t>GSM Send Data over HTTP</t>
+  </si>
+  <si>
+    <t>Re do GSM Send Data over HTTP for 100 times</t>
+  </si>
+  <si>
+    <t>When µC receive error ack message from any GSM AT cmd, then µC send same cmd 5 time if still no get OK ack message. After 5 retries, APP notifies "APP_HANDLE_ERROR: GSM_ERROR_DEV_ACK" by Callback function. And stuck in same stage because There are no Error handling form Application's side</t>
+  </si>
+  <si>
+    <t>Re do Error Handling - GSM_ERROR_DEV_UNRESPONSIVE for 100 times</t>
+  </si>
+  <si>
+    <t>When Unresponsive error comes, at that time a nofity callback to the App side and reset and deint &amp; init all module and work from the APP init.</t>
+  </si>
+  <si>
+    <t>For any HTTP status other than 200:
 Resend the same data</t>
   </si>
   <si>
-    <t>Retransmits the data</t>
-  </si>
-  <si>
-    <t>GPS MTK3339 Module</t>
-  </si>
-  <si>
-    <t>Observations</t>
-  </si>
-  <si>
-    <t>Observation Details</t>
-  </si>
-  <si>
-    <t>test</t>
+    <t>Error Handling - GSM_HTTP_INIT_ERROR</t>
+  </si>
+  <si>
+    <t>Re do Error Handling - GSM_HTTP_INIT_ERROR for 50 times</t>
+  </si>
+  <si>
+    <t>For HTTP_INIT error, this a exception case in AT HTTP cmd. Cause, First time GSM module return OK ack message at initilize of HTTP_INIT cmd. But incase if HTTP_INIT cmd fire again before it HTTP_Terminate cmd fire. Then It will return ERROR ack message.</t>
+  </si>
+  <si>
+    <t>For HTTP_INIT error, this a exception case in AT HTTP cmd. Cause, First time GSM module return OK ack message at initilize of HTTP_INIT cmd. But incase if HTTP_INIT cmd fire again before it HTTP_Terminate cmd fire. Then It will return ERROR ack message. So HTTP_INIT return OK thes its good otherwise, we have to HTTP_Terminate first and then HTTP_INIT again and do the rest process.</t>
+  </si>
+  <si>
+    <t>Yse it work fine as our desired result.</t>
+  </si>
+  <si>
+    <t>When GSM_HTTP_INIT called, GSM return ok if it’s a first time otherwise it return ERROR and process goes to the HTTP_Terminate and init again.</t>
+  </si>
+  <si>
+    <t>GSM_HTTPDATA Response Error</t>
+  </si>
+  <si>
+    <t>Re do GSM_HTTPDATA 50 times</t>
+  </si>
+  <si>
+    <t>After make the Json data string, Call the AT+HTTPDATA=data_len,send_time and enter the wait for DOWNLOAD ack and after that send the Json Data to GSM module</t>
+  </si>
+  <si>
+    <t>Send AT+HTTPDATA=data_len,send_time , wait for DOWNLOAD, then send DATA wait for OK. Then do the remaing tasks</t>
+  </si>
+  <si>
+    <t>This process fine but sometime get Usart Read Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When Usart Read error comes in that case deinit &amp; init the usart and pause at that state and wait for time out of send data and OK ack. Then again execute the same CMD and </t>
+  </si>
+  <si>
+    <t>When ERROR_USART comes that time change the state GSM_DEV_USART_ERROR or GSM_HTTP_USART_ERROR or GPS_MTK3339_USART_ERROR. And then deinit and init the USART</t>
+  </si>
+  <si>
+    <t>Error Handling - ERROR_USART</t>
+  </si>
+  <si>
+    <t>Re do Error Handling - ERROR_USART 10 times</t>
+  </si>
+  <si>
+    <t>After deinit and init the usart, the process works fine.</t>
+  </si>
+  <si>
+    <t>When Usart error comes that time process goes to usart error handler state, and deint &amp; init the specific usart and do the same process again.</t>
+  </si>
+  <si>
+    <t>I make a harcode usart error, for the reason of that hardcode error, process goes to usart error handler and deinit &amp; init the usart and again execute the same process. This Usart error handle run for 10 time if still usart not woring right, after 10 time retries app been notify by callback and then print only "[../src/app.c:650] APP_HANDLE_ERROR: GSM_ERROR_USART".</t>
+  </si>
+  <si>
+    <t>GPS_SENSOR_READ</t>
+  </si>
+  <si>
+    <t>Re do GPS_SENSOR_READ 10 times</t>
+  </si>
+  <si>
+    <t>Read GPS data, Parse RMC and GGA data</t>
+  </si>
+  <si>
+    <t>Read GPS data strings cut the only RMC data string, then check data string Active or Void Data string. If void again read till time out. Then parse that RMC string. If data is active then read GGA from Bunch of GPS data string. And parse it and notify App by call back.</t>
+  </si>
+  <si>
+    <t>Start Timer for read, then check data string Active or Void Data string. If void again read till time out. Then parse that RMC string. If data is active then read GGA from Bunch of GPS data string. And parse it and notify App by call back.</t>
+  </si>
+  <si>
+    <t>When ERROR_USART comes that time change the state GPS_MTK3339_USART_ERROR. And then deinit and init the USART</t>
+  </si>
+  <si>
+    <t>I make a harcode usart error, for the reason of that hardcode error, process goes to usart error handler and deinit &amp; init the usart and again execute the same process. This Usart error handle run for 10 time if still usart not woring right, after 10 time retries app been notify by callback and then print only "[../src/app.c:59] GPS_ERROR_USART
+[../src/app.c:63] ERR MSG: USART Error in GPS MTK3339. STATE ID: 2". and this print again and again. So, Possible reason is, we forget to set_gps_process_stat(false); in GPS_IDLE state.</t>
   </si>
 </sst>
 </file>
@@ -136,7 +270,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -149,8 +283,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -186,11 +326,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -216,8 +365,35 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,213 +689,347 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:G13"/>
+  <dimension ref="A2:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" style="13" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="9" t="s">
+      <c r="H2" s="11"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="1:7" ht="63.75">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:8" ht="120">
       <c r="A4" s="3">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7">
+    </row>
+    <row r="5" spans="1:8" ht="63.75">
       <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="D5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="3">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="51">
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" ht="76.5">
       <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="63.75">
+      <c r="F7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="63.75">
       <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="4"/>
+      <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="51">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" ht="51">
       <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="25.5">
+      <c r="F9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="25.5">
       <c r="A10" s="3">
         <v>7</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" ht="102">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="63.75">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="102">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="1:7" ht="51">
-      <c r="A13" s="6">
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+    </row>
+    <row r="15" spans="1:8" s="17" customFormat="1" ht="76.5">
+      <c r="A15" s="16">
         <v>1</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B15" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="E15" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="51">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8" t="s">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E16" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:7" ht="140.25">
+      <c r="A17" s="3">
+        <v>10</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A12:G12"/>
+    <mergeCell ref="A14:G14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Github issues created based on the report of the previous commit and issue ID updated in this file
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -298,22 +298,6 @@
     <t>When GPS module not present that time µC try to read data from GPS module. And failed</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">When GPS module not present that time µC try to read data from GPS module. And failed for unresponsive, and after tring 10 time µC return </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
-    </r>
-  </si>
-  <si>
     <t>Redo, try to hit unknown link from GSM_module  100 time</t>
   </si>
   <si>
@@ -372,13 +356,31 @@
   </si>
   <si>
     <t>Read ADC data and store into variable.</t>
+  </si>
+  <si>
+    <t>When GPS module not present that time µC try to read data from GPS module. And failed for unresponsive, and after tring 10 time µC return "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
+  </si>
+  <si>
+    <t>Github Issue ID</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>#4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,8 +411,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,8 +444,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -472,20 +486,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -511,15 +517,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -538,9 +535,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -550,8 +544,30 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -846,21 +862,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="13" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="10" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="10" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="24" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8">
@@ -870,56 +887,61 @@
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="11"/>
+      <c r="H2" s="9" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
-      <c r="A4" s="3">
+      <c r="A4" s="18">
         <v>1</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="20" t="s">
         <v>24</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="99" customHeight="1">
@@ -944,6 +966,7 @@
       <c r="G5" s="5" t="s">
         <v>60</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" spans="1:8" ht="25.5">
       <c r="A6" s="3">
@@ -959,26 +982,30 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A7" s="3">
+      <c r="A7" s="18">
         <v>4</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
+      <c r="C7" s="20"/>
+      <c r="D7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="20" t="s">
         <v>31</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="89.25" customHeight="1">
@@ -989,7 +1016,7 @@
         <v>14</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>15</v>
@@ -1001,8 +1028,9 @@
         <v>39</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>74</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" ht="66" customHeight="1">
       <c r="A9" s="3">
@@ -1026,8 +1054,9 @@
       <c r="G9" s="5" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="51">
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" ht="38.25">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1035,7 +1064,7 @@
         <v>18</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>34</v>
@@ -1044,11 +1073,12 @@
         <v>19</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>80</v>
-      </c>
+      <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="117" customHeight="1">
       <c r="A11" s="3">
@@ -1072,6 +1102,7 @@
       <c r="G11" s="5" t="s">
         <v>40</v>
       </c>
+      <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="63.75">
       <c r="A12" s="3">
@@ -1095,6 +1126,7 @@
       <c r="G12" s="5" t="s">
         <v>46</v>
       </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="131.25" customHeight="1">
       <c r="A13" s="3">
@@ -1118,59 +1150,65 @@
       <c r="G13" s="5" t="s">
         <v>52</v>
       </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="131.25" customHeight="1">
-      <c r="A14" s="3">
+      <c r="A14" s="18">
         <v>11</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5" t="s">
+      <c r="G14" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>77</v>
+      <c r="H14" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-    </row>
-    <row r="16" spans="1:8" s="16" customFormat="1" ht="76.5">
-      <c r="A16" s="15">
+      <c r="B15" s="15"/>
+      <c r="C15" s="15"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" s="13" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A16" s="12">
         <v>1</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="12" t="s">
         <v>53</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="14" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" ht="51">
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:8" ht="51">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1186,8 +1224,9 @@
       </c>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="153">
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" ht="170.25" customHeight="1">
       <c r="A18" s="3">
         <v>10</v>
       </c>
@@ -1209,107 +1248,119 @@
       <c r="G18" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-    </row>
-    <row r="20" spans="1:7" s="13" customFormat="1" ht="81" customHeight="1">
-      <c r="A20" s="18">
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="17"/>
+      <c r="F19" s="17"/>
+      <c r="G19" s="17"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" s="10" customFormat="1" ht="88.5" customHeight="1">
+      <c r="A20" s="22">
         <v>1</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="5" t="s">
+      <c r="F20" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="20" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" ht="68.25" customHeight="1">
-      <c r="A21" s="3">
+      <c r="H20" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="108.75" customHeight="1">
+      <c r="A21" s="18">
         <v>2</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F21" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="114.75">
-      <c r="A22" s="3">
+      <c r="G21" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="135">
+      <c r="A22" s="18">
         <v>3</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="19" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="D22" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="F22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="F22" s="5" t="s">
+      <c r="G22" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="51">
+      <c r="H22" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="64.5" customHeight="1">
       <c r="A23" s="3">
         <v>4</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>89</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5" t="s">
-        <v>91</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="H23" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Created issue in github and added issue ID for Sl.No. 10
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>#4</t>
+  </si>
+  <si>
+    <t>#15</t>
   </si>
 </sst>
 </file>
@@ -535,6 +538,27 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -542,27 +566,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -862,9 +865,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -876,7 +879,7 @@
     <col min="5" max="5" width="45.85546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" style="10" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="24" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="21" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -907,37 +910,37 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
-      <c r="A4" s="18">
+      <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -985,23 +988,23 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A7" s="18">
+      <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="17" t="s">
         <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1153,19 +1156,19 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="131.25" customHeight="1">
-      <c r="A14" s="18">
+      <c r="A14" s="15">
         <v>11</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="17" t="s">
         <v>76</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1173,15 +1176,15 @@
       </c>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
+      <c r="B15" s="22"/>
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" s="13" customFormat="1" ht="92.25" customHeight="1">
@@ -1206,7 +1209,7 @@
       <c r="G16" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="23"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8" ht="51">
       <c r="A17" s="6">
@@ -1227,61 +1230,63 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="170.25" customHeight="1">
-      <c r="A18" s="3">
+      <c r="A18" s="15">
         <v>10</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="17" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="H18" s="1"/>
+      <c r="H18" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="17"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" s="10" customFormat="1" ht="88.5" customHeight="1">
-      <c r="A20" s="22">
+      <c r="A20" s="19">
         <v>1</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="17" t="s">
         <v>66</v>
       </c>
       <c r="H20" s="9" t="s">
@@ -1289,25 +1294,25 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="108.75" customHeight="1">
-      <c r="A21" s="18">
+      <c r="A21" s="15">
         <v>2</v>
       </c>
-      <c r="B21" s="19" t="s">
+      <c r="B21" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="C21" s="20" t="s">
+      <c r="C21" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E21" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G21" s="17" t="s">
         <v>92</v>
       </c>
       <c r="H21" s="1" t="s">
@@ -1315,25 +1320,25 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="135">
-      <c r="A22" s="18">
+      <c r="A22" s="15">
         <v>3</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="16" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="17" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="E22" s="20" t="s">
+      <c r="E22" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="17" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G22" s="17" t="s">
         <v>82</v>
       </c>
       <c r="H22" s="1" t="s">

</xml_diff>

<commit_message>
Add new bug report HTTP_POST_DATA, AT+COPS?
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Stuck at APP_HANDLE_ERROR : GSM_ERROR_DEV_ACK</t>
   </si>
   <si>
-    <t>Usart read error shows rendomly when µC try to read CMD_ACK. Prints only "APP_HANDLE_ERROR: GSM_ERROR_DEV_ACK". There are no Error handling form Application's side. Getting Error ACK message,at AT+CSTT="www","","". Getting error ack message after running GPS init(block) 7 times at interval of 10sec.</t>
-  </si>
-  <si>
-    <t>Usart read error rendomly, General Exception</t>
-  </si>
-  <si>
     <t>Allocate required memory
 Init USART
 Sends sequence of AT commands and receive the responses</t>
@@ -152,9 +146,6 @@
     <t>For HTTP_INIT error, this a exception case in AT HTTP cmd. Cause, First time GSM module return OK ack message at initilize of HTTP_INIT cmd. But incase if HTTP_INIT cmd fire again before it HTTP_Terminate cmd fire. Then It will return ERROR ack message. So HTTP_INIT return OK thes its good otherwise, we have to HTTP_Terminate first and then HTTP_INIT again and do the rest process.</t>
   </si>
   <si>
-    <t>Yse it work fine as our desired result.</t>
-  </si>
-  <si>
     <t>When GSM_HTTP_INIT called, GSM return ok if it’s a first time otherwise it return ERROR and process goes to the HTTP_Terminate and init again.</t>
   </si>
   <si>
@@ -216,8 +207,152 @@
 [../src/app.c:63] ERR MSG: USART Error in GPS MTK3339. STATE ID: 2". and this print again and again. So, Possible reason is, we forget to set_gps_process_stat(false); in GPS_IDLE state.</t>
   </si>
   <si>
+    <t>Battery Low</t>
+  </si>
+  <si>
+    <t>When battery became low</t>
+  </si>
+  <si>
+    <t>When device battery become low, then device complete the ongoing process and notify the user for battery is being low.</t>
+  </si>
+  <si>
+    <t>When device battery become low, complete the ongoing process and notify the user for battery is being low.</t>
+  </si>
+  <si>
+    <t>When battery become low, GPS &amp; GSM module's power goes down from their's require Volt supply limit. So, they stop, But still µC running and try to communicate with those module.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When GSM stop working, than µC try communicate and getting unresponsive. </t>
+  </si>
+  <si>
+    <t>GPS_Module_Not Attach</t>
+  </si>
+  <si>
+    <t>When GPS_Module_Not Attach</t>
+  </si>
+  <si>
+    <t>Check GPS module attach or not then read data from module</t>
+  </si>
+  <si>
+    <t>If module present then read data from module otherwish show a notification</t>
+  </si>
+  <si>
+    <t>When GPS module not present that time µC try to read data from GPS module. And failed</t>
+  </si>
+  <si>
+    <t>Redo, try to hit unknown link from GSM_module  100 time</t>
+  </si>
+  <si>
+    <t>SIM_card not present</t>
+  </si>
+  <si>
+    <t>Faild at AT+COPS? "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
+  </si>
+  <si>
+    <t>Re do Error Handling - GSM_ERROR_HTTP_SERVER_ERROR for 50 times</t>
+  </si>
+  <si>
+    <t>Right now, http server code other than 200, re-init all and start from the beginning. From AT cmd.</t>
+  </si>
+  <si>
+    <t>Right now, http server code other than 200, re-init all and start from the beginning. From AT cmd, and again read GPS data and then try to send.</t>
+  </si>
+  <si>
+    <t>ADC_Humidity_and_Battery</t>
+  </si>
+  <si>
+    <t>Need delay at read adc buff for getting correct data data.</t>
+  </si>
+  <si>
+    <t>When use delay at read adc buff, the adc read value is correct. But there is a mistake at "while(bsp_harmony_adc_samples_available()==true); ", mistake is, we need to wait for sample as true otherwise wait on that step. So, solution is, we have to use "while(bsp_harmony_adc_samples_available()!=true);" and wait for sampling, in that case, no need delay at adc read buff..</t>
+  </si>
+  <si>
+    <t>After read and validate GPS data GPRMC data Read ADC data at APP_READ_SENSOR state</t>
+  </si>
+  <si>
+    <t>Both module attached and read one after one module</t>
+  </si>
+  <si>
+    <t>iqwsiot_firmware Module_&amp;_ADC</t>
+  </si>
+  <si>
+    <t>memory leaks</t>
+  </si>
+  <si>
+    <t>Check memory leaks every time after completing one full cycle process, in Http 200 and Http 500.</t>
+  </si>
+  <si>
+    <t>Check memory leaks every time after completing one full cycle process, show the memory leaks in the program.</t>
+  </si>
+  <si>
+    <t>Check memory leaks every time after completing of full cycle process,</t>
+  </si>
+  <si>
+    <t>Check memory leaks every time after completing one full cycle process, show the memory leaks in the program.  in case of full cycle of Http 200 and Http 500, there are no memory leaks.</t>
+  </si>
+  <si>
+    <t>Read ADC data and store into variable.</t>
+  </si>
+  <si>
+    <t>When GPS module not present that time µC try to read data from GPS module. And failed for unresponsive, and after tring 10 time µC return "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
+  </si>
+  <si>
+    <t>Github Issue ID</t>
+  </si>
+  <si>
+    <t>#12</t>
+  </si>
+  <si>
+    <t>#13</t>
+  </si>
+  <si>
+    <t>#14</t>
+  </si>
+  <si>
+    <t>#4</t>
+  </si>
+  <si>
+    <t>#15</t>
+  </si>
+  <si>
+    <t>Getting ACK Usart read error at state of GSM_HTTP_HTTP_POST_DATA</t>
+  </si>
+  <si>
+    <t>ACK Usart read error at GSM_HTTP_HTTP_POST_DATA</t>
+  </si>
+  <si>
+    <t>At error time again send that same command</t>
+  </si>
+  <si>
+    <t>At error time again send that same command, but the data of GSM_HTTP_HTTP_POST_DATA state's CMD, is a 2nd part of AT+HTTPDATA.</t>
+  </si>
+  <si>
+    <t>In GSM_HTTP_HTTP_POST_DATA, this is a 2nd part of a command 'AT+HTTPDATA'. So, when Usart read error comes, at that time we have to fire first 'AT+HTTPDATA' cmd in GSM_HTTP_HTTP_SET_POST_DATA_CMD state then GSM_HTTP_HTTP_POST_DATA,</t>
+  </si>
+  <si>
+    <t>When sim card is not present  at AT+COPS?, get "General Exception Data bus error (cause=7, addr=9d0039d4)." When sim card not present ACK of AT+COPS? Is "\r\n+COPS: 1/0\r\n\r\nOK\r\n". So, when sim card not present, that time there no error handling on ACK of AT+COPS?.</t>
+  </si>
+  <si>
+    <t>No ERROR Handling and NULL pointer checking at AT cmd ACK parsing.</t>
+  </si>
+  <si>
+    <t>Yes it work fine as our desired result.</t>
+  </si>
+  <si>
+    <t>Yes it work fine as our desired result. But some getting "General Exception Data bus error"</t>
+  </si>
+  <si>
+    <t>When this kind of error occure, at that time, deinit and init usart and fire the same command</t>
+  </si>
+  <si>
+    <t>Usart read error shows randomly when µC try to read CMD_ACK. Prints only "APP_HANDLE_ERROR: GSM_ERROR_DEV_ACK". There are no Error handling form Application's side. Getting Error ACK message,at AT+CSTT="www","","". Getting error ack message after running GPS init(block) 7 times at interval of 10sec.</t>
+  </si>
+  <si>
+    <t>Usart read error randomly, General Exception</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Observation count = 258, Usart read error shows rendomly. 
+      <t xml:space="preserve">Observation count = 258, Usart read error shows randomly. 
 </t>
     </r>
     <r>
@@ -264,126 +399,12 @@
       <t xml:space="preserve"> </t>
     </r>
   </si>
-  <si>
-    <t>Battery Low</t>
-  </si>
-  <si>
-    <t>When battery became low</t>
-  </si>
-  <si>
-    <t>When device battery become low, then device complete the ongoing process and notify the user for battery is being low.</t>
-  </si>
-  <si>
-    <t>When device battery become low, complete the ongoing process and notify the user for battery is being low.</t>
-  </si>
-  <si>
-    <t>When battery become low, GPS &amp; GSM module's power goes down from their's require Volt supply limit. So, they stop, But still µC running and try to communicate with those module.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When GSM stop working, than µC try communicate and getting unresponsive. </t>
-  </si>
-  <si>
-    <t>GPS_Module_Not Attach</t>
-  </si>
-  <si>
-    <t>When GPS_Module_Not Attach</t>
-  </si>
-  <si>
-    <t>Check GPS module attach or not then read data from module</t>
-  </si>
-  <si>
-    <t>If module present then read data from module otherwish show a notification</t>
-  </si>
-  <si>
-    <t>When GPS module not present that time µC try to read data from GPS module. And failed</t>
-  </si>
-  <si>
-    <t>Redo, try to hit unknown link from GSM_module  100 time</t>
-  </si>
-  <si>
-    <t>Yse it work fine as our desired result. But some getting "General Exception Data bus error"</t>
-  </si>
-  <si>
-    <t>SIM_card not present</t>
-  </si>
-  <si>
-    <t>Faild at AT+COPS? "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
-  </si>
-  <si>
-    <t>When sim card is not present  at AT+COPS?, get "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
-  </si>
-  <si>
-    <t>Re do Error Handling - GSM_ERROR_HTTP_SERVER_ERROR for 50 times</t>
-  </si>
-  <si>
-    <t>Right now, http server code other than 200, re-init all and start from the beginning. From AT cmd.</t>
-  </si>
-  <si>
-    <t>Right now, http server code other than 200, re-init all and start from the beginning. From AT cmd, and again read GPS data and then try to send.</t>
-  </si>
-  <si>
-    <t>ADC_Humidity_and_Battery</t>
-  </si>
-  <si>
-    <t>Need delay at read adc buff for getting correct data data.</t>
-  </si>
-  <si>
-    <t>When use delay at read adc buff, the adc read value is correct. But there is a mistake at "while(bsp_harmony_adc_samples_available()==true); ", mistake is, we need to wait for sample as true otherwise wait on that step. So, solution is, we have to use "while(bsp_harmony_adc_samples_available()!=true);" and wait for sampling, in that case, no need delay at adc read buff..</t>
-  </si>
-  <si>
-    <t>After read and validate GPS data GPRMC data Read ADC data at APP_READ_SENSOR state</t>
-  </si>
-  <si>
-    <t>Both module attached and read one after one module</t>
-  </si>
-  <si>
-    <t>iqwsiot_firmware Module_&amp;_ADC</t>
-  </si>
-  <si>
-    <t>memory leaks</t>
-  </si>
-  <si>
-    <t>Check memory leaks every time after completing one full cycle process, in Http 200 and Http 500.</t>
-  </si>
-  <si>
-    <t>Check memory leaks every time after completing one full cycle process, show the memory leaks in the program.</t>
-  </si>
-  <si>
-    <t>Check memory leaks every time after completing of full cycle process,</t>
-  </si>
-  <si>
-    <t>Check memory leaks every time after completing one full cycle process, show the memory leaks in the program.  in case of full cycle of Http 200 and Http 500, there are no memory leaks.</t>
-  </si>
-  <si>
-    <t>Read ADC data and store into variable.</t>
-  </si>
-  <si>
-    <t>When GPS module not present that time µC try to read data from GPS module. And failed for unresponsive, and after tring 10 time µC return "General Exception Data bus error (cause=7, addr=9d0039d4)."</t>
-  </si>
-  <si>
-    <t>Github Issue ID</t>
-  </si>
-  <si>
-    <t>#12</t>
-  </si>
-  <si>
-    <t>#13</t>
-  </si>
-  <si>
-    <t>#14</t>
-  </si>
-  <si>
-    <t>#4</t>
-  </si>
-  <si>
-    <t>#15</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +438,25 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -494,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -506,18 +546,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -542,9 +576,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
@@ -567,6 +598,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -863,23 +906,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:H23"/>
+  <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A18" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" style="10" customWidth="1"/>
-    <col min="4" max="4" width="34.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="45.85546875" style="10" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="45.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="21" customWidth="1"/>
+    <col min="1" max="1" width="6.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" style="8" customWidth="1"/>
+    <col min="4" max="4" width="34.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.85546875" style="8" customWidth="1"/>
+    <col min="6" max="6" width="38.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="45.7109375" style="8" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="18" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -887,64 +930,64 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="E2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H2" s="9" t="s">
-        <v>93</v>
+      <c r="H2" s="7" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
-      <c r="A4" s="15">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="F4" s="18" t="s">
+      <c r="E4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="17" t="s">
-        <v>24</v>
+      <c r="G4" s="14" t="s">
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="99" customHeight="1">
@@ -954,20 +997,20 @@
       <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>60</v>
+      <c r="F5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>105</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -976,39 +1019,39 @@
         <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" ht="106.5" customHeight="1">
+      <c r="A7" s="13">
+        <v>4</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row r="7" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A7" s="15">
-        <v>4</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>31</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="89.25" customHeight="1">
@@ -1018,20 +1061,20 @@
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>73</v>
+      <c r="F8" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>101</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -1042,20 +1085,20 @@
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>33</v>
+      <c r="F9" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -1066,20 +1109,20 @@
       <c r="B10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="C10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>79</v>
+      <c r="F10" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>73</v>
       </c>
       <c r="H10" s="1"/>
     </row>
@@ -1088,22 +1131,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="E11" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="F11" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -1112,22 +1155,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="F12" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="G12" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E12" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="G12" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -1136,242 +1179,280 @@
         <v>10</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" ht="131.25" customHeight="1">
+      <c r="A14" s="13">
+        <v>11</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="25" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A15" s="22">
+        <v>12</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="24"/>
+    </row>
+    <row r="16" spans="1:8" s="25" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A16" s="22">
+        <v>13</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="24"/>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" s="11" customFormat="1" ht="92.25" customHeight="1">
+      <c r="A18" s="10">
+        <v>1</v>
+      </c>
+      <c r="B18" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="17"/>
+    </row>
+    <row r="19" spans="1:8" ht="51">
+      <c r="A19" s="5">
+        <v>1</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" ht="170.25" customHeight="1">
+      <c r="A20" s="13">
+        <v>10</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="G13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" ht="131.25" customHeight="1">
-      <c r="A14" s="15">
-        <v>11</v>
-      </c>
-      <c r="B14" s="16" t="s">
+      <c r="F20" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" s="8" customFormat="1" ht="88.5" customHeight="1">
+      <c r="A22" s="16">
+        <v>1</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="108.75" customHeight="1">
+      <c r="A23" s="13">
+        <v>2</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="135">
+      <c r="A24" s="13">
+        <v>3</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="17"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17" t="s">
+      <c r="C24" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="F24" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G24" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="22"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" s="13" customFormat="1" ht="92.25" customHeight="1">
-      <c r="A16" s="12">
-        <v>1</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="20"/>
-    </row>
-    <row r="17" spans="1:8" ht="51">
-      <c r="A17" s="6">
-        <v>1</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" ht="170.25" customHeight="1">
-      <c r="A18" s="15">
-        <v>10</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="C18" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="23" t="s">
-        <v>85</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" s="10" customFormat="1" ht="88.5" customHeight="1">
-      <c r="A20" s="19">
-        <v>1</v>
-      </c>
-      <c r="B20" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>66</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="108.75" customHeight="1">
-      <c r="A21" s="15">
-        <v>2</v>
-      </c>
-      <c r="B21" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C21" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="135">
-      <c r="A22" s="15">
-        <v>3</v>
-      </c>
-      <c r="B22" s="16" t="s">
+      <c r="H24" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="64.5" customHeight="1">
+      <c r="A25" s="3">
+        <v>4</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C25" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="D22" s="17" t="s">
-        <v>83</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="64.5" customHeight="1">
-      <c r="A23" s="3">
-        <v>4</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="1"/>
+      <c r="H25" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A15:G15"/>
-    <mergeCell ref="A19:G19"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="A21:G21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added List of parser_functions
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -398,6 +398,9 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>List of parser_function -&gt; parse_gprs_status, parse_sim_number, parse_imsi, parse_imei, parse_model, parse_mfg_name, parse_service_provider_info, parse_operator_info, parse_httpaction_status, parse_HTTPREAD_status</t>
   </si>
 </sst>
 </file>
@@ -590,6 +593,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -598,18 +613,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -908,9 +911,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -953,15 +956,15 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
@@ -1218,54 +1221,56 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="25" customFormat="1" ht="131.25" customHeight="1">
-      <c r="A15" s="22">
+    <row r="15" spans="1:8" s="22" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A15" s="19">
         <v>12</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="20" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="20" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="20" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="24"/>
-    </row>
-    <row r="16" spans="1:8" s="25" customFormat="1" ht="131.25" customHeight="1">
-      <c r="A16" s="22">
+      <c r="H15" s="21"/>
+    </row>
+    <row r="16" spans="1:8" s="22" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A16" s="19">
         <v>13</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="24"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G16" s="20"/>
+      <c r="H16" s="21"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="92.25" customHeight="1">
@@ -1337,15 +1342,15 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" s="8" customFormat="1" ht="88.5" customHeight="1">

</xml_diff>

<commit_message>
Sprint #2 test cases updated
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="test_cases" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="sprint1" sheetId="4" r:id="rId1"/>
+    <sheet name="sprint2" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -402,12 +402,37 @@
   <si>
     <t>List of parser_function -&gt; parse_gprs_status, parse_sim_number, parse_imsi, parse_imei, parse_model, parse_mfg_name, parse_service_provider_info, parse_operator_info, parse_httpaction_status, parse_HTTPREAD_status</t>
   </si>
+  <si>
+    <t>Query and check if a sensor is attached or not</t>
+  </si>
+  <si>
+    <t>Full Functionality test for normal &amp; failure conditions</t>
+  </si>
+  <si>
+    <t>Run for 5 hours
+Pre-Auth
+Auth
+Post Data</t>
+  </si>
+  <si>
+    <t>Data to be posted successfully to the server.
+Error to be notified with log and LED</t>
+  </si>
+  <si>
+    <t>#17</t>
+  </si>
+  <si>
+    <t>Sensors not attached Error Handling</t>
+  </si>
+  <si>
+    <t>If any sensor module is not attached then application should notify error via Log &amp; LED. All other operations should continue normally</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -464,8 +489,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -493,6 +525,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -533,11 +570,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -576,12 +614,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
@@ -614,9 +646,26 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -911,9 +960,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -925,7 +974,7 @@
     <col min="5" max="5" width="45.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="38.85546875" style="8" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.7109375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="17.42578125" style="18" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" style="16" customWidth="1"/>
     <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -956,37 +1005,37 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
-      <c r="A4" s="13">
+      <c r="A4" s="24">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="25" t="s">
         <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1034,23 +1083,23 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A7" s="13">
+      <c r="A7" s="24">
         <v>4</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="25"/>
+      <c r="D7" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="25" t="s">
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1202,75 +1251,75 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="131.25" customHeight="1">
-      <c r="A14" s="13">
+      <c r="A14" s="24">
         <v>11</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="14"/>
-      <c r="F14" s="14" t="s">
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="25" t="s">
         <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="22" customFormat="1" ht="131.25" customHeight="1">
-      <c r="A15" s="19">
+    <row r="15" spans="1:8" s="20" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A15" s="17">
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>94</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="F15" s="20" t="s">
+      <c r="F15" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="H15" s="21"/>
-    </row>
-    <row r="16" spans="1:8" s="22" customFormat="1" ht="131.25" customHeight="1">
-      <c r="A16" s="19">
+      <c r="H15" s="19"/>
+    </row>
+    <row r="16" spans="1:8" s="20" customFormat="1" ht="131.25" customHeight="1">
+      <c r="A16" s="17">
         <v>13</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="18" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20" t="s">
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="H16" s="21"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="92.25" customHeight="1">
@@ -1295,7 +1344,7 @@
       <c r="G18" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="H18" s="17"/>
+      <c r="H18" s="15"/>
     </row>
     <row r="19" spans="1:8" ht="51">
       <c r="A19" s="5">
@@ -1316,25 +1365,25 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="170.25" customHeight="1">
-      <c r="A20" s="13">
+      <c r="A20" s="24">
         <v>10</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="25" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="25" t="s">
         <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1342,37 +1391,37 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="24" t="s">
+      <c r="A21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" s="8" customFormat="1" ht="88.5" customHeight="1">
-      <c r="A22" s="16">
+      <c r="A22" s="14">
         <v>1</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="14" t="s">
+      <c r="C22" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="F22" s="14" t="s">
+      <c r="F22" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="13" t="s">
         <v>62</v>
       </c>
       <c r="H22" s="7" t="s">
@@ -1380,51 +1429,49 @@
       </c>
     </row>
     <row r="23" spans="1:8" ht="108.75" customHeight="1">
-      <c r="A23" s="13">
+      <c r="A23" s="17">
         <v>2</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="14" t="s">
+      <c r="C23" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="18" t="s">
         <v>86</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>90</v>
-      </c>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" ht="135">
-      <c r="A24" s="13">
+      <c r="A24" s="24">
         <v>3</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="14" t="s">
+      <c r="C24" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="14" t="s">
+      <c r="E24" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="14" t="s">
+      <c r="F24" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="14" t="s">
+      <c r="G24" s="25" t="s">
         <v>76</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1466,13 +1513,91 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="25.5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="51">
+      <c r="A2" s="27">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
+        <v>107</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
+    </row>
+    <row r="3" spans="1:8" ht="51">
+      <c r="A3" s="27">
+        <v>2</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28" t="s">
+        <v>110</v>
+      </c>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="19" t="s">
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Memory Leak in tokenize_response
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -426,6 +426,27 @@
   </si>
   <si>
     <t>If any sensor module is not attached then application should notify error via Log &amp; LED. All other operations should continue normally</t>
+  </si>
+  <si>
+    <t>Memory_leak</t>
+  </si>
+  <si>
+    <t>Full phase running, with preauth &amp; then post data</t>
+  </si>
+  <si>
+    <t>Show the memory leak status.</t>
+  </si>
+  <si>
+    <t>Yes, there's a memory leak at the time of GSM response tokenize.</t>
+  </si>
+  <si>
+    <t>Firmware tasks check memory leak</t>
+  </si>
+  <si>
+    <t>In line number 146/147 of tokenize_response(char* ack_str) of gsm_sim800_utility.c. Memory leak shows. Log_file_name of memory_leak testing result "mem_leak_sprint2.txt"</t>
+  </si>
+  <si>
+    <t>#18</t>
   </si>
 </sst>
 </file>
@@ -575,7 +596,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -637,6 +658,18 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -646,22 +679,21 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -670,6 +702,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF700000"/>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -961,7 +999,7 @@
   <dimension ref="A2:H25"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
@@ -1005,37 +1043,37 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
-      <c r="A4" s="24">
+      <c r="A4" s="21">
         <v>1</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="C4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="22" t="s">
         <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1083,23 +1121,23 @@
       <c r="H6" s="1"/>
     </row>
     <row r="7" spans="1:8" ht="106.5" customHeight="1">
-      <c r="A7" s="24">
+      <c r="A7" s="21">
         <v>4</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25" t="s">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="25" t="s">
+      <c r="E7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="25" t="s">
+      <c r="G7" s="22" t="s">
         <v>29</v>
       </c>
       <c r="H7" s="1" t="s">
@@ -1251,19 +1289,19 @@
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" ht="131.25" customHeight="1">
-      <c r="A14" s="24">
+      <c r="A14" s="21">
         <v>11</v>
       </c>
-      <c r="B14" s="25" t="s">
+      <c r="B14" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25" t="s">
+      <c r="C14" s="22"/>
+      <c r="D14" s="22"/>
+      <c r="E14" s="22"/>
+      <c r="F14" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="25" t="s">
+      <c r="G14" s="22" t="s">
         <v>98</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1311,15 +1349,15 @@
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="92.25" customHeight="1">
@@ -1365,25 +1403,25 @@
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" ht="170.25" customHeight="1">
-      <c r="A20" s="24">
+      <c r="A20" s="21">
         <v>10</v>
       </c>
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="C20" s="25" t="s">
+      <c r="C20" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="D20" s="25" t="s">
+      <c r="D20" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="E20" s="25" t="s">
+      <c r="E20" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F20" s="25" t="s">
+      <c r="F20" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="22" t="s">
         <v>56</v>
       </c>
       <c r="H20" s="1" t="s">
@@ -1391,15 +1429,15 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="22" t="s">
+      <c r="A21" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" s="8" customFormat="1" ht="88.5" customHeight="1">
@@ -1453,25 +1491,25 @@
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" ht="135">
-      <c r="A24" s="24">
+      <c r="A24" s="21">
         <v>3</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="C24" s="25" t="s">
+      <c r="C24" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="25" t="s">
+      <c r="F24" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="22" t="s">
         <v>76</v>
       </c>
       <c r="H24" s="1" t="s">
@@ -1513,86 +1551,113 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="1" max="1" width="5.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="28" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51">
-      <c r="A2" s="27">
+      <c r="A2" s="24">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24" t="s">
         <v>107</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
       <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" ht="51">
-      <c r="A3" s="27">
+      <c r="A3" s="24">
         <v>2</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="24" t="s">
         <v>109</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="19" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="31" t="s">
         <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="32" customFormat="1" ht="75">
+      <c r="A4" s="13">
+        <v>3</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HTTP Stat 601 observation updated in full functionality test.
</commit_message>
<xml_diff>
--- a/iqwsiot_firmware_testing.xlsx
+++ b/iqwsiot_firmware_testing.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="122">
   <si>
     <t>Sl. No.</t>
   </si>
@@ -447,6 +447,9 @@
   </si>
   <si>
     <t>#18</t>
+  </si>
+  <si>
+    <t>1. HTTP stat: 601 occurs after long duration operation</t>
   </si>
 </sst>
 </file>
@@ -596,7 +599,7 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -670,6 +673,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -679,20 +688,17 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1043,15 +1049,15 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="1"/>
     </row>
     <row r="4" spans="1:8" ht="135.75" customHeight="1">
@@ -1349,15 +1355,15 @@
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="25" t="s">
+      <c r="A17" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" s="11" customFormat="1" ht="92.25" customHeight="1">
@@ -1429,15 +1435,15 @@
       </c>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>79</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" s="8" customFormat="1" ht="88.5" customHeight="1">
@@ -1553,51 +1559,51 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="16.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.85546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="43.42578125" style="28" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41.42578125" style="28" customWidth="1"/>
-    <col min="8" max="8" width="9.28515625" style="28" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="28"/>
+    <col min="1" max="1" width="5.85546875" style="31" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="16.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="43.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41.42578125" style="25" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" style="31" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="25"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="25.5">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="7" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="51">
-      <c r="A2" s="24">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
@@ -1612,10 +1618,10 @@
       </c>
       <c r="F2" s="24"/>
       <c r="G2" s="24"/>
-      <c r="H2" s="29"/>
+      <c r="H2" s="32"/>
     </row>
     <row r="3" spans="1:8" ht="51">
-      <c r="A3" s="24">
+      <c r="A3" s="30">
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
@@ -1628,14 +1634,16 @@
       <c r="E3" s="24" t="s">
         <v>110</v>
       </c>
-      <c r="F3" s="24"/>
+      <c r="F3" s="24" t="s">
+        <v>121</v>
+      </c>
       <c r="G3" s="24"/>
-      <c r="H3" s="31" t="s">
+      <c r="H3" s="33" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="32" customFormat="1" ht="75">
-      <c r="A4" s="13">
+    <row r="4" spans="1:8" s="26" customFormat="1" ht="75">
+      <c r="A4" s="14">
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
@@ -1656,7 +1664,7 @@
       <c r="G4" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="14" t="s">
         <v>120</v>
       </c>
     </row>

</xml_diff>